<commit_message>
basic hard code chatbot
</commit_message>
<xml_diff>
--- a/Manually_Extracted_data.xlsx
+++ b/Manually_Extracted_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuvra\OneDrive\Desktop\KASHI\Forage_financial_document_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBF002E-E3E5-47C1-BF15-9A2F4E7ECCEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6D45C3-4D73-468C-8130-7BB3E2C0BECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E3D57D30-FC78-45AD-9212-B61D79A127F7}"/>
   </bookViews>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
-    <t xml:space="preserve"> Net Income</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Total Assets</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>Total Revenue ($ millions)</t>
+  </si>
+  <si>
+    <t>Net Income</t>
   </si>
 </sst>
 </file>
@@ -430,7 +430,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -445,30 +445,30 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>2023</v>
@@ -491,7 +491,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>2022</v>
@@ -514,7 +514,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>2021</v>
@@ -537,7 +537,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>2023</v>
@@ -560,7 +560,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>2022</v>
@@ -583,7 +583,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>2021</v>
@@ -606,7 +606,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>2023</v>
@@ -629,7 +629,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>2022</v>
@@ -652,7 +652,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10">
         <v>2021</v>

</xml_diff>